<commit_message>
Carga del Taller 2
</commit_message>
<xml_diff>
--- a/MONITOR/2021-2/Taller1/Estudiantes.xlsx
+++ b/MONITOR/2021-2/Taller1/Estudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UJ\UJ2021-01\Monitorias\revisionTrabajos\MONITOR\2021-2\Taller1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\revisionTrabajos\MONITOR\2021-2\Taller1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE86CEB3-0421-421C-8AC4-3830EEAF1FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7B64D3-94C4-431A-82DD-36C76E4EFEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taller3" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Taller3!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Estudiante</t>
   </si>
@@ -125,6 +128,12 @@
   </si>
   <si>
     <t>No vi el taller</t>
+  </si>
+  <si>
+    <t>PROMEDIO</t>
+  </si>
+  <si>
+    <t>CONVERSIÓN</t>
   </si>
 </sst>
 </file>
@@ -402,7 +411,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -415,6 +423,12 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -437,12 +451,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4365,9 +4374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -4380,23 +4389,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1" thickBot="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="19" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="20" t="s">
         <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="46.5" customHeight="1">
@@ -4415,17 +4430,17 @@
       <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="20"/>
+      <c r="G3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
@@ -4443,49 +4458,73 @@
       <c r="E4" s="6">
         <v>10</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="8">
+        <f>+SUM(C4:E4)/3</f>
+        <v>10</v>
+      </c>
+      <c r="H4" s="21">
+        <f>+G4*5/10</f>
+        <v>5</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="14">
         <v>10</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="14">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="14">
         <v>10</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="14">
         <v>10</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="8">
+        <f t="shared" ref="G5:G21" si="0">+SUM(C5:E5)/3</f>
+        <v>9.9333333333333336</v>
+      </c>
+      <c r="H5" s="21">
+        <f t="shared" ref="H5:H22" si="1">+G5*5/10</f>
+        <v>4.9666666666666668</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="14">
         <v>9.6</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="14">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="14">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="14">
         <v>9.8000000000000007</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="H6" s="21">
+        <f t="shared" si="1"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1">
       <c r="A7" s="7" t="s">
@@ -4503,9 +4542,17 @@
       <c r="E7" s="6">
         <v>8</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>9.2666666666666675</v>
+      </c>
+      <c r="H7" s="21">
+        <f t="shared" si="1"/>
+        <v>4.6333333333333337</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -4523,18 +4570,26 @@
       <c r="E8" s="6">
         <v>10</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
+        <v>9.9333333333333336</v>
+      </c>
+      <c r="H8" s="21">
+        <f t="shared" si="1"/>
+        <v>4.9666666666666668</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="13">
         <v>1</v>
       </c>
       <c r="D9" s="6">
@@ -4543,11 +4598,19 @@
       <c r="E9" s="6">
         <v>6</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="H9" s="21">
+        <f t="shared" si="1"/>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1">
       <c r="A10" s="7" t="s">
@@ -4565,18 +4628,26 @@
       <c r="E10" s="6">
         <v>8</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>9.2666666666666675</v>
+      </c>
+      <c r="H10" s="21">
+        <f t="shared" si="1"/>
+        <v>4.6333333333333337</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:14" ht="28.5">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>1</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <v>1</v>
       </c>
       <c r="D11" s="6">
@@ -4585,11 +4656,19 @@
       <c r="E11" s="6">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="H11" s="21">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1">
       <c r="A12" s="7" t="s">
@@ -4607,9 +4686,17 @@
       <c r="E12" s="6">
         <v>10</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H12" s="21">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1">
       <c r="A13" s="7" t="s">
@@ -4627,9 +4714,17 @@
       <c r="E13" s="6">
         <v>10</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="8">
+        <f t="shared" si="0"/>
+        <v>9.9333333333333336</v>
+      </c>
+      <c r="H13" s="21">
+        <f t="shared" si="1"/>
+        <v>4.9666666666666668</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1">
       <c r="A14" s="7" t="s">
@@ -4647,23 +4742,39 @@
       <c r="E14" s="6">
         <v>7</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="8">
+        <f t="shared" si="0"/>
+        <v>8.6</v>
+      </c>
+      <c r="H14" s="21">
+        <f t="shared" si="1"/>
+        <v>4.3</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1">
       <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="11" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="G15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1">
       <c r="A16" s="7" t="s">
@@ -4681,9 +4792,17 @@
       <c r="E16" s="6">
         <v>9.9</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="8">
+        <f t="shared" si="0"/>
+        <v>9.9666666666666668</v>
+      </c>
+      <c r="H16" s="21">
+        <f t="shared" si="1"/>
+        <v>4.9833333333333334</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1">
       <c r="A17" s="7" t="s">
@@ -4701,10 +4820,17 @@
       <c r="E17" s="6">
         <v>10</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="8"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H17" s="21">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="15">
       <c r="A18" s="7" t="s">
@@ -4722,9 +4848,17 @@
       <c r="E18" s="6">
         <v>10</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="8">
+        <f t="shared" si="0"/>
+        <v>9.7999999999999989</v>
+      </c>
+      <c r="H18" s="21">
+        <f t="shared" si="1"/>
+        <v>4.8999999999999995</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="15">
       <c r="A19" s="7" t="s">
@@ -4742,9 +4876,17 @@
       <c r="E19" s="6">
         <v>10</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H19" s="21">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="15">
       <c r="A20" s="7" t="s">
@@ -4762,9 +4904,17 @@
       <c r="E20" s="6">
         <v>9.6</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="8">
+        <f t="shared" si="0"/>
+        <v>9.2000000000000011</v>
+      </c>
+      <c r="H20" s="21">
+        <f t="shared" si="1"/>
+        <v>4.6000000000000005</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="17.25" customHeight="1">
       <c r="A21" s="7" t="s">
@@ -4782,9 +4932,17 @@
       <c r="E21" s="6">
         <v>8.4</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="8">
+        <f t="shared" si="0"/>
+        <v>9.2666666666666657</v>
+      </c>
+      <c r="H21" s="21">
+        <f t="shared" si="1"/>
+        <v>4.6333333333333329</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="A22" s="7" t="s">
@@ -4802,11 +4960,19 @@
       <c r="E22" s="6">
         <v>10</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
+      <c r="G22" s="8">
+        <f>+SUM(C22:E22)/3</f>
+        <v>10</v>
+      </c>
+      <c r="H22" s="21">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>